<commit_message>
Lots of updates for Sirenum, Out There
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="150" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="G4">
-        <v>15000</v>
+        <v>40</v>
       </c>
       <c r="H4" t="s">
         <v>6</v>
@@ -793,7 +793,7 @@
         <v>18</v>
       </c>
       <c r="G5">
-        <v>0.11</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -823,7 +823,7 @@
       </c>
       <c r="G8" s="3">
         <f>G4*(3.14*G5/30)^2</f>
-        <v>1.9883526666666675</v>
+        <v>0.63101439999999998</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>20</v>
@@ -845,7 +845,7 @@
       </c>
       <c r="G9" s="5">
         <f>G8/9.81</f>
-        <v>0.20268630648997629</v>
+        <v>6.4323588175331292E-2</v>
       </c>
       <c r="H9" s="3"/>
     </row>
@@ -858,7 +858,7 @@
       </c>
       <c r="G10" s="3">
         <f>(G4)*2*3.14*G5/60</f>
-        <v>172.7</v>
+        <v>5.024</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>23</v>
@@ -968,7 +968,7 @@
         <v>27</v>
       </c>
       <c r="B20" s="19">
-        <v>3.472222222222222E-3</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="B22" s="3">
         <f>B20*9.81*B21*60*60</f>
-        <v>147150</v>
+        <v>58860.000000000007</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>23</v>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="B23" s="3">
         <f>1/(SQRT(1-B22^2/B16^2))</f>
-        <v>1.0000001204617615</v>
+        <v>1.0000000192738789</v>
       </c>
       <c r="C23" s="3"/>
       <c r="F23" s="3" t="s">
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B24" s="9">
         <f>B22/B23/1000</f>
-        <v>147.14998227405394</v>
+        <v>58.859998865539517</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>35</v>
@@ -1061,7 +1061,7 @@
       <c r="A25" s="7"/>
       <c r="B25" s="3">
         <f>B24/B17</f>
-        <v>4.9083950695668916E-4</v>
+        <v>1.9633582264947947E-4</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>30</v>
@@ -1083,7 +1083,7 @@
       </c>
       <c r="B26" s="12">
         <f>0.5*(B20*9.81*(B21*3600)^2)/1000</f>
-        <v>317844000</v>
+        <v>127137600.00000001</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>15</v>
@@ -1103,7 +1103,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="10">
         <f>B26/149597870.7</f>
-        <v>2.1246559092902921</v>
+        <v>0.8498623637161169</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>33</v>
@@ -1126,7 +1126,7 @@
       </c>
       <c r="B29" s="12">
         <f>B28*3600*B24+B26</f>
-        <v>4026023553.3061595</v>
+        <v>1610409571.4115958</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>15</v>
@@ -1142,7 +1142,7 @@
       <c r="A30" s="7"/>
       <c r="B30" s="3">
         <f>B29/149597870.7</f>
-        <v>26.912305198379805</v>
+        <v>10.7649230826358</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>33</v>
@@ -1186,7 +1186,7 @@
       </c>
       <c r="B32" s="10">
         <f>B30+B27</f>
-        <v>29.036961107670098</v>
+        <v>11.614785446351917</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>33</v>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="B35" s="9">
         <f>(B20*9.81*B31*60*60/1000)+B24</f>
-        <v>294.29998227405395</v>
+        <v>117.71999886553952</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Updates for Out There
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3060" yWindow="260" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -727,7 +727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="G4">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
         <v>6</v>
@@ -793,7 +793,7 @@
         <v>18</v>
       </c>
       <c r="G5">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -823,7 +823,7 @@
       </c>
       <c r="G8" s="3">
         <f>G4*(3.14*G5/30)^2</f>
-        <v>0.63101439999999998</v>
+        <v>0.21033813333333343</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>20</v>
@@ -845,7 +845,7 @@
       </c>
       <c r="G9" s="5">
         <f>G8/9.81</f>
-        <v>6.4323588175331292E-2</v>
+        <v>2.1441196058443773E-2</v>
       </c>
       <c r="H9" s="3"/>
     </row>
@@ -858,7 +858,7 @@
       </c>
       <c r="G10" s="3">
         <f>(G4)*2*3.14*G5/60</f>
-        <v>5.024</v>
+        <v>2.512</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>23</v>
@@ -1092,8 +1092,8 @@
         <v>51</v>
       </c>
       <c r="G26" s="9">
-        <f>9.81*G20*LOG(G18/G19)/1000</f>
-        <v>302.85120466799697</v>
+        <f>9.81*G20*LN(G18/G19)/1000</f>
+        <v>697.34066926381854</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>35</v>

</xml_diff>